<commit_message>
Add password age, login age, policy violation checks, and risk scoring
</commit_message>
<xml_diff>
--- a/data/user_access_inventory.xlsx
+++ b/data/user_access_inventory.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaive\IT-Access-Audit\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2F0A57-28BE-4D95-BF2E-4A6A8F93AC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="68">
   <si>
     <t>Username</t>
   </si>
@@ -164,16 +170,70 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>New Column Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Password Age (days)</t>
+  </si>
+  <si>
+    <t>=TODAY() - [Password Last Changed]</t>
+  </si>
+  <si>
+    <t>Login Age (days)</t>
+  </si>
+  <si>
+    <t>=TODAY() - [Last Login]</t>
+  </si>
+  <si>
+    <t>Violation: Password Age</t>
+  </si>
+  <si>
+    <t>=IF([Password Age]&gt;90, "YES", "NO")</t>
+  </si>
+  <si>
+    <t>Violation: MFA</t>
+  </si>
+  <si>
+    <t>=IF([MFA Enabled]="N", "YES", "NO")</t>
+  </si>
+  <si>
+    <t>Violation: Inactive</t>
+  </si>
+  <si>
+    <t>=IF([Login Age]&gt;60, "YES", "NO")</t>
+  </si>
+  <si>
+    <t>Violation: Terminated</t>
+  </si>
+  <si>
+    <t>=IF([Termination Date]&lt;&gt;"", "YES", "NO")</t>
+  </si>
+  <si>
+    <t>Violation: Admin Review</t>
+  </si>
+  <si>
+    <t>=IF(AND([Admin Access]="Y", [Login Age]&gt;30), "YES", "NO")</t>
+  </si>
+  <si>
+    <t>Risk Score</t>
+  </si>
+  <si>
+    <t>=SUM(...based on how many "YES" entries * weights...)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +248,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -225,25 +290,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -281,7 +363,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -315,6 +397,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -349,9 +432,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -524,14 +608,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="49" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="6" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="24.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,7 +648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -579,8 +670,14 @@
       <c r="H2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="J2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -602,8 +699,14 @@
       <c r="H3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="J3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -625,8 +728,14 @@
       <c r="H4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="J4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -648,8 +757,14 @@
       <c r="H5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="J5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -671,8 +786,14 @@
       <c r="H6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="J6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -694,8 +815,14 @@
       <c r="H7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="J7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -717,8 +844,14 @@
       <c r="H8" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="J8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="100" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -740,8 +873,14 @@
       <c r="H9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="J9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="100" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -763,8 +902,14 @@
       <c r="H10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="J10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -787,7 +932,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -813,7 +958,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -836,7 +981,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -859,7 +1004,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -885,7 +1030,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -908,7 +1053,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -931,7 +1076,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -954,7 +1099,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -977,7 +1122,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1003,7 +1148,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1029,7 +1174,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1052,7 +1197,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1075,7 +1220,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1098,7 +1243,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1121,7 +1266,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1144,7 +1289,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1167,7 +1312,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1190,7 +1335,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1213,7 +1358,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1236,7 +1381,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
Add policy violation flags and total risk scoring columns
</commit_message>
<xml_diff>
--- a/data/user_access_inventory.xlsx
+++ b/data/user_access_inventory.xlsx
@@ -8,19 +8,54 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaive\IT-Access-Audit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2F0A57-28BE-4D95-BF2E-4A6A8F93AC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4895ACF4-367C-4291-A6C0-80B7D8F25A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="67">
   <si>
     <t>Username</t>
   </si>
@@ -220,10 +255,7 @@
     <t>=IF(AND([Admin Access]="Y", [Login Age]&gt;30), "YES", "NO")</t>
   </si>
   <si>
-    <t>Risk Score</t>
-  </si>
-  <si>
-    <t>=SUM(...based on how many "YES" entries * weights...)</t>
+    <t>Total Risk Score</t>
   </si>
 </sst>
 </file>
@@ -233,7 +265,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,10 +331,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -611,18 +643,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="49" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="5" max="6" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
     <col min="11" max="11" width="24.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -648,7 +681,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -677,7 +710,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -699,14 +732,14 @@
       <c r="H3" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -728,14 +761,14 @@
       <c r="H4" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -757,14 +790,14 @@
       <c r="H5" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="J5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="29">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -786,14 +819,14 @@
       <c r="H6" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="J6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -815,14 +848,14 @@
       <c r="H7" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="29">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -844,14 +877,14 @@
       <c r="H8" t="s">
         <v>48</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="100" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="37.5">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -873,14 +906,14 @@
       <c r="H9" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="100" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -902,14 +935,15 @@
       <c r="H10" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K10" s="4" t="e" cm="1">
+        <f t="array" ref="K10">(MFA * 3) + (Password Age * 2) + (Inactive * 1) + (Terminated * 3) + (Admin Review * 2)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -932,7 +966,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -958,7 +992,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -981,7 +1015,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1004,7 +1038,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1030,7 +1064,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1053,7 +1087,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1076,7 +1110,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1099,7 +1133,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1122,7 +1156,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1148,7 +1182,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1174,7 +1208,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1197,7 +1231,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1220,7 +1254,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1243,7 +1277,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1266,7 +1300,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1289,7 +1323,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1312,7 +1346,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1335,7 +1369,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1358,7 +1392,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1381,7 +1415,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
Add audit scoring columns and violation logic
</commit_message>
<xml_diff>
--- a/data/user_access_inventory.xlsx
+++ b/data/user_access_inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaive\IT-Access-Audit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4895ACF4-367C-4291-A6C0-80B7D8F25A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147B72E9-A06C-4174-B24E-817B5D524CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,30 +32,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="58">
   <si>
     <t>Username</t>
   </si>
@@ -207,55 +185,28 @@
     <t>N</t>
   </si>
   <si>
-    <t>New Column Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Password Age (days)</t>
   </si>
   <si>
-    <t>=TODAY() - [Password Last Changed]</t>
-  </si>
-  <si>
-    <t>Login Age (days)</t>
-  </si>
-  <si>
-    <t>=TODAY() - [Last Login]</t>
-  </si>
-  <si>
-    <t>Violation: Password Age</t>
-  </si>
-  <si>
-    <t>=IF([Password Age]&gt;90, "YES", "NO")</t>
-  </si>
-  <si>
     <t>Violation: MFA</t>
   </si>
   <si>
-    <t>=IF([MFA Enabled]="N", "YES", "NO")</t>
-  </si>
-  <si>
     <t>Violation: Inactive</t>
   </si>
   <si>
-    <t>=IF([Login Age]&gt;60, "YES", "NO")</t>
-  </si>
-  <si>
     <t>Violation: Terminated</t>
   </si>
   <si>
-    <t>=IF([Termination Date]&lt;&gt;"", "YES", "NO")</t>
-  </si>
-  <si>
     <t>Violation: Admin Review</t>
   </si>
   <si>
-    <t>=IF(AND([Admin Access]="Y", [Login Age]&gt;30), "YES", "NO")</t>
-  </si>
-  <si>
-    <t>Total Risk Score</t>
+    <t xml:space="preserve">	Login Age (days)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Violation: Password Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Total Risk Score</t>
   </si>
 </sst>
 </file>
@@ -322,20 +273,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,21 +595,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I5" sqref="I1:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="5" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.90625" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
     <col min="11" max="11" width="24.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:16" ht="58">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -680,8 +635,32 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="I1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -703,14 +682,25 @@
       <c r="H2" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="25">
+      <c r="I2">
+        <f ca="1">TODAY() - E2</f>
+        <v>114</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2">
+        <f>IF(D2="N", 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2">
+        <f>IF(AND(H2="Y", J2&gt;30), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="5"/>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -732,14 +722,29 @@
       <c r="H3" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="J3" s="3">
+        <f ca="1">TODAY() - F2</f>
+        <v>25</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <f ca="1">IF(I2&gt;90, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="M3" s="3">
+        <f>IF(J2&gt;60, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <f>IF(ISNUMBER(G2), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="3">
+        <f>(K2*3)+(L2*2)+(M2*1)+(N2*3)+(O2*2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -761,14 +766,10 @@
       <c r="H4" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="25">
+      <c r="J4" s="4"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -790,14 +791,10 @@
       <c r="H5" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="29">
+      <c r="J5" s="4"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -819,14 +816,10 @@
       <c r="H6" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="25">
+      <c r="J6" s="4"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -848,14 +841,10 @@
       <c r="H7" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="29">
+      <c r="J7" s="4"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -877,14 +866,10 @@
       <c r="H8" t="s">
         <v>48</v>
       </c>
-      <c r="J8" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="37.5">
+      <c r="J8" s="4"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -906,14 +891,10 @@
       <c r="H9" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="J9" s="4"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -935,15 +916,10 @@
       <c r="H10" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="K10" s="4" t="e" cm="1">
-        <f t="array" ref="K10">(MFA * 3) + (Password Age * 2) + (Inactive * 1) + (Terminated * 3) + (Admin Review * 2)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="J10" s="4"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -965,8 +941,9 @@
       <c r="H11" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -992,7 +969,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1015,7 +992,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1038,7 +1015,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1064,7 +1041,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1087,7 +1064,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:19">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1110,7 +1087,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:19">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1133,7 +1110,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:19">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1156,7 +1133,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:19">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1182,7 +1159,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:19">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1208,7 +1185,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:19">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1231,7 +1208,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:19">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1254,7 +1231,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:19">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1277,7 +1254,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:19">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1300,7 +1277,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:19">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1323,7 +1300,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:19">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1346,7 +1323,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:19">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1369,7 +1346,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:19">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1392,7 +1369,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:19">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1414,8 +1391,12 @@
       <c r="H30" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="S30" t="str">
+        <f>TRIM(CLEAN(G2))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1437,8 +1418,17 @@
       <c r="H31" t="s">
         <v>48</v>
       </c>
+      <c r="Q31" t="str">
+        <f>TRIM(CLEAN(G2))</f>
+        <v/>
+      </c>
+      <c r="R31" t="str">
+        <f>TRIM(CLEAN(G2))</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>